<commit_message>
NatRes to zero and modified reformat indexes
</commit_message>
<xml_diff>
--- a/src/reformat_exiobase/mappings/map_GTAP_format.xlsx
+++ b/src/reformat_exiobase/mappings/map_GTAP_format.xlsx
@@ -22,17 +22,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="38">
+  <si>
+    <t xml:space="preserve">CI_imp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All_sectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">∑</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CI_dom</t>
+  </si>
   <si>
     <t xml:space="preserve">CI</t>
   </si>
   <si>
-    <t xml:space="preserve">All_sectors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">∑</t>
-  </si>
-  <si>
     <t xml:space="preserve">∑∑</t>
   </si>
   <si>
@@ -67,6 +73,12 @@
   </si>
   <si>
     <t xml:space="preserve">Prod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax_imp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax_dom</t>
   </si>
   <si>
     <t xml:space="preserve">FBCF Imp</t>
@@ -226,11 +238,11 @@
   </sheetPr>
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.96"/>
@@ -254,7 +266,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>1</v>
@@ -262,7 +274,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>2</v>
@@ -270,79 +282,79 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>2</v>
@@ -350,23 +362,23 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>2</v>
@@ -374,79 +386,79 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>2</v>
@@ -454,7 +466,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>1</v>
@@ -462,7 +474,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>2</v>
@@ -470,7 +482,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>1</v>
@@ -478,7 +490,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>2</v>
@@ -486,31 +498,31 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>2</v>
@@ -518,23 +530,23 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>2</v>
@@ -542,23 +554,23 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>2</v>
@@ -566,31 +578,31 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>2</v>
@@ -598,18 +610,18 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -634,33 +646,33 @@
       <selection pane="topLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,46 +689,46 @@
         <v>2</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -741,39 +753,39 @@
       <selection pane="topLeft" activeCell="R10" activeCellId="0" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,55 +802,55 @@
         <v>2</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="Q2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="T2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reported energy consumption by Government to Households
</commit_message>
<xml_diff>
--- a/src/reformat_exiobase/mappings/map_GTAP_format.xlsx
+++ b/src/reformat_exiobase/mappings/map_GTAP_format.xlsx
@@ -238,11 +238,11 @@
   </sheetPr>
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.96"/>
@@ -646,7 +646,7 @@
       <selection pane="topLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -753,7 +753,7 @@
       <selection pane="topLeft" activeCell="R10" activeCellId="0" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>